<commit_message>
Added more comments and refreshed ThreshE and added comments for it
</commit_message>
<xml_diff>
--- a/Observations/2022-02-19/07in/Targets/A21/Shifts/ha/2022-02-19_A21_ha_shifts.xlsx
+++ b/Observations/2022-02-19/07in/Targets/A21/Shifts/ha/2022-02-19_A21_ha_shifts.xlsx
@@ -56,8 +56,8 @@
   <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="true"/>
-    <col min="2" max="2" width="2.85546875" customWidth="true"/>
+    <col min="1" max="1" width="2.85546875" customWidth="true"/>
+    <col min="2" max="2" width="3.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -70,74 +70,74 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B2" s="0">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B8" s="0">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>